<commit_message>
Enable economic retirements of coal plants due to ETS by requiring plants to return a profit in SoFCtMbCtPR
</commit_message>
<xml_diff>
--- a/InputData/elec/CRpUNL/Cap Ret per Unit Net Loss.xlsx
+++ b/InputData/elec/CRpUNL/Cap Ret per Unit Net Loss.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\elec\CRpUNL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\elec\CRpUNL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784A2D67-3F06-44C3-AAA2-D5E31B535A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF3C6A0-25B6-4FC6-946A-F1A284FBA868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="15" windowWidth="23010" windowHeight="13770" xr2:uid="{67B50A2A-83E2-40E1-A966-DC033ADD8EBF}"/>
+    <workbookView xWindow="30900" yWindow="2100" windowWidth="21600" windowHeight="12525" activeTab="1" xr2:uid="{67B50A2A-83E2-40E1-A966-DC033ADD8EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -533,18 +533,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B7A547-DAFD-4CBC-90C6-A86A1413C282}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -552,42 +552,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -604,16 +604,16 @@
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -621,7 +621,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -629,7 +629,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -637,15 +637,15 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -653,7 +653,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -669,7 +669,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -677,7 +677,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -685,7 +685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -693,7 +693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -701,7 +701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -709,7 +709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -717,7 +717,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -725,7 +725,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -733,7 +733,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -741,7 +741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -749,7 +749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -765,7 +765,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -773,7 +773,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -781,7 +781,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -789,7 +789,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -797,7 +797,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>27</v>
       </c>
@@ -805,7 +805,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Updates to eps-us commit #e782024
</commit_message>
<xml_diff>
--- a/InputData/elec/CRpUNL/Cap Ret per Unit Net Loss.xlsx
+++ b/InputData/elec/CRpUNL/Cap Ret per Unit Net Loss.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\elec\CRpUNL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CRpUNL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784A2D67-3F06-44C3-AAA2-D5E31B535A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789C4A85-6A1E-41E5-8FBD-A2A66D513898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="15" windowWidth="23010" windowHeight="13770" xr2:uid="{67B50A2A-83E2-40E1-A966-DC033ADD8EBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{67B50A2A-83E2-40E1-A966-DC033ADD8EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -605,7 +605,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updates to eps-us commit #e090f27
</commit_message>
<xml_diff>
--- a/InputData/elec/CRpUNL/Cap Ret per Unit Net Loss.xlsx
+++ b/InputData/elec/CRpUNL/Cap Ret per Unit Net Loss.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CRpUNL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us-analysis\InputData\elec\CRpUNL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789C4A85-6A1E-41E5-8FBD-A2A66D513898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6567EA64-6F7D-43AE-A26B-B09A74E72F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{67B50A2A-83E2-40E1-A966-DC033ADD8EBF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{67B50A2A-83E2-40E1-A966-DC033ADD8EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -183,18 +183,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -209,14 +203,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,7 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B7A547-DAFD-4CBC-90C6-A86A1413C282}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -604,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +619,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.03</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -634,7 +627,8 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.03</v>
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -642,7 +636,8 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.03</v>
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -650,14 +645,15 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.03</v>
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>0</v>
       </c>
     </row>
@@ -666,7 +662,8 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.03</v>
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -674,14 +671,15 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.03</v>
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9">
         <v>0</v>
       </c>
     </row>
@@ -689,7 +687,7 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10">
         <v>0</v>
       </c>
     </row>
@@ -697,7 +695,7 @@
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11">
         <v>0</v>
       </c>
     </row>
@@ -705,7 +703,7 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12">
         <v>0</v>
       </c>
     </row>
@@ -714,7 +712,8 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>0.03</v>
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -722,7 +721,8 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>0.03</v>
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -730,14 +730,15 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>0.03</v>
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16">
         <v>0</v>
       </c>
     </row>
@@ -745,7 +746,7 @@
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17">
         <v>0</v>
       </c>
     </row>
@@ -753,7 +754,7 @@
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18">
         <v>0</v>
       </c>
     </row>
@@ -761,56 +762,63 @@
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="4">
-        <v>0.03</v>
+      <c r="B19">
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="4">
-        <v>0.03</v>
+      <c r="B20">
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="4">
-        <v>0.03</v>
+      <c r="B21">
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="4">
-        <v>0.03</v>
+      <c r="B22">
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="4">
-        <v>0.03</v>
+      <c r="B23">
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="4">
-        <v>0.03</v>
+      <c r="B24">
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="4">
-        <v>0.03</v>
+      <c r="B25">
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ref 2020 capacity calibration
</commit_message>
<xml_diff>
--- a/InputData/elec/CRpUNL/Cap Ret per Unit Net Loss.xlsx
+++ b/InputData/elec/CRpUNL/Cap Ret per Unit Net Loss.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\elec\CRpUNL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF3C6A0-25B6-4FC6-946A-F1A284FBA868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6513CD7-70B6-47A7-A068-794EFC0B7343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30900" yWindow="2100" windowWidth="21600" windowHeight="12525" activeTab="1" xr2:uid="{67B50A2A-83E2-40E1-A966-DC033ADD8EBF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{67B50A2A-83E2-40E1-A966-DC033ADD8EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -534,7 +534,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -605,7 +605,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -626,7 +626,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -634,7 +634,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -642,7 +642,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>3.5000000000000003E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -705,8 +705,8 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="4">
-        <v>0</v>
+      <c r="B12">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>